<commit_message>
Split video, and looped them to play back to back
</commit_message>
<xml_diff>
--- a/Capstone_GhostBikesQueens.xlsx
+++ b/Capstone_GhostBikesQueens.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amartini/Desktop/Bri_DH/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amartini/Desktop/Bri_DH/Capstone/Ghost_Bikes_of_Queens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDAA6A1-87AC-3046-8213-C9B55D2B0C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E26AEBE-44DF-1341-B3C8-432EF9FA1BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{8D5CAD35-F28B-9440-8FBE-C76FE2793AC5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{8D5CAD35-F28B-9440-8FBE-C76FE2793AC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2014,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28876565-45B2-9045-A729-6D7F2448CFF8}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S65" sqref="S65"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>